<commit_message>
Improved model structure and started statistics display
</commit_message>
<xml_diff>
--- a/Project2/dataset/parsed/test.xlsx
+++ b/Project2/dataset/parsed/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64F650A-30B5-46D5-9606-9FA23435CA29}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8002417A-741A-4EA3-805A-46012AB8D042}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3354,11 +3354,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A989" workbookViewId="0">
+      <selection activeCell="A1002" sqref="A1002:C3528"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="88.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -14899,7 +14902,7 @@
         <v>4</v>
       </c>
       <c r="C962" t="str">
-        <f t="shared" ref="C962:C1001" si="15">IF(B962&gt;5,"Positive","Negative")</f>
+        <f t="shared" ref="C962:C1025" si="15">IF(B962&gt;5,"Positive","Negative")</f>
         <v>Negative</v>
       </c>
     </row>

</xml_diff>